<commit_message>
config(displayModeBar = F) to save time
</commit_message>
<xml_diff>
--- a/extraVariables.xlsx
+++ b/extraVariables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27022"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="0" windowWidth="21000" windowHeight="13980"/>
+    <workbookView xWindow="11060" yWindow="0" windowWidth="14180" windowHeight="13980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -694,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:AZ55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -711,11 +711,12 @@
     <col min="7" max="7" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" customWidth="1"/>
     <col min="11" max="11" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="52" width="8.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:52">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -750,7 +751,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:52">
       <c r="A2" s="2">
         <v>363</v>
       </c>
@@ -785,7 +786,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:52">
       <c r="A3" s="2">
         <v>365</v>
       </c>
@@ -820,7 +821,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:52">
       <c r="A4" s="2">
         <v>460</v>
       </c>
@@ -855,7 +856,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="17" customFormat="1">
+    <row r="5" spans="1:52" s="17" customFormat="1">
       <c r="A5" s="2">
         <v>465</v>
       </c>
@@ -889,8 +890,49 @@
       <c r="K5" s="9">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="15"/>
+      <c r="AD5" s="15"/>
+      <c r="AE5" s="15"/>
+      <c r="AF5" s="15"/>
+      <c r="AG5" s="15"/>
+      <c r="AH5" s="15"/>
+      <c r="AI5" s="15"/>
+      <c r="AJ5" s="15"/>
+      <c r="AK5" s="15"/>
+      <c r="AL5" s="15"/>
+      <c r="AM5" s="15"/>
+      <c r="AN5" s="15"/>
+      <c r="AO5" s="15"/>
+      <c r="AP5" s="15"/>
+      <c r="AQ5" s="15"/>
+      <c r="AR5" s="15"/>
+      <c r="AS5" s="15"/>
+      <c r="AT5" s="15"/>
+      <c r="AU5" s="15"/>
+      <c r="AV5" s="15"/>
+      <c r="AW5" s="15"/>
+      <c r="AX5" s="15"/>
+      <c r="AY5" s="15"/>
+      <c r="AZ5" s="15"/>
+    </row>
+    <row r="6" spans="1:52">
       <c r="A6" s="2">
         <v>362</v>
       </c>
@@ -925,7 +967,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:52">
       <c r="A7" s="2">
         <v>427</v>
       </c>
@@ -960,7 +1002,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:52">
       <c r="A8" s="4">
         <v>391</v>
       </c>
@@ -995,7 +1037,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:52">
       <c r="A9" s="11">
         <v>421</v>
       </c>
@@ -1030,7 +1072,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:52">
       <c r="A10" s="4">
         <v>430</v>
       </c>
@@ -1065,7 +1107,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:52">
       <c r="A11" s="4">
         <v>482</v>
       </c>
@@ -1100,7 +1142,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="15" customFormat="1">
+    <row r="12" spans="1:52" s="15" customFormat="1">
       <c r="A12" s="4">
         <v>367</v>
       </c>
@@ -1135,7 +1177,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="15" customFormat="1">
+    <row r="13" spans="1:52" s="15" customFormat="1">
       <c r="A13" s="4">
         <v>429</v>
       </c>
@@ -1170,7 +1212,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="15" customFormat="1">
+    <row r="14" spans="1:52" s="15" customFormat="1">
       <c r="A14" s="4">
         <v>368</v>
       </c>
@@ -1205,7 +1247,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="15" customFormat="1">
+    <row r="15" spans="1:52" s="15" customFormat="1">
       <c r="A15" s="2">
         <v>467</v>
       </c>
@@ -1240,7 +1282,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="15" customFormat="1">
+    <row r="16" spans="1:52" s="15" customFormat="1">
       <c r="A16" s="2">
         <v>406</v>
       </c>
@@ -1275,7 +1317,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="15" customFormat="1">
+    <row r="17" spans="1:52" s="15" customFormat="1">
       <c r="A17" s="2">
         <v>410</v>
       </c>
@@ -1310,7 +1352,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:52">
       <c r="A18" s="2">
         <v>434</v>
       </c>
@@ -1345,7 +1387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:52">
       <c r="A19" s="2">
         <v>436</v>
       </c>
@@ -1380,7 +1422,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="18" customFormat="1">
+    <row r="20" spans="1:52" s="18" customFormat="1">
       <c r="A20" s="4">
         <v>371</v>
       </c>
@@ -1414,8 +1456,49 @@
       <c r="K20" s="9">
         <v>9.3000000000000007</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="15"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="15"/>
+      <c r="AC20" s="15"/>
+      <c r="AD20" s="15"/>
+      <c r="AE20" s="15"/>
+      <c r="AF20" s="15"/>
+      <c r="AG20" s="15"/>
+      <c r="AH20" s="15"/>
+      <c r="AI20" s="15"/>
+      <c r="AJ20" s="15"/>
+      <c r="AK20" s="15"/>
+      <c r="AL20" s="15"/>
+      <c r="AM20" s="15"/>
+      <c r="AN20" s="15"/>
+      <c r="AO20" s="15"/>
+      <c r="AP20" s="15"/>
+      <c r="AQ20" s="15"/>
+      <c r="AR20" s="15"/>
+      <c r="AS20" s="15"/>
+      <c r="AT20" s="15"/>
+      <c r="AU20" s="15"/>
+      <c r="AV20" s="15"/>
+      <c r="AW20" s="15"/>
+      <c r="AX20" s="15"/>
+      <c r="AY20" s="15"/>
+      <c r="AZ20" s="15"/>
+    </row>
+    <row r="21" spans="1:52">
       <c r="A21" s="11">
         <v>385</v>
       </c>
@@ -1450,7 +1533,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:52">
       <c r="A22" s="11">
         <v>382</v>
       </c>
@@ -1485,7 +1568,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:52">
       <c r="A23" s="4">
         <v>425</v>
       </c>
@@ -1520,7 +1603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:52">
       <c r="A24" s="4">
         <v>438</v>
       </c>
@@ -1555,7 +1638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="15" customFormat="1">
+    <row r="25" spans="1:52" s="15" customFormat="1">
       <c r="A25" s="4">
         <v>449</v>
       </c>
@@ -1590,7 +1673,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:52">
       <c r="A26" s="2">
         <v>407</v>
       </c>
@@ -1625,7 +1708,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:52">
       <c r="A27" s="2">
         <v>447</v>
       </c>
@@ -1660,7 +1743,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:52">
       <c r="A28" s="2">
         <v>471</v>
       </c>
@@ -1695,7 +1778,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:52">
       <c r="A29" s="2">
         <v>477</v>
       </c>
@@ -1730,7 +1813,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:52">
       <c r="A30" s="2">
         <v>374</v>
       </c>
@@ -1765,7 +1848,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:52">
       <c r="A31" s="2">
         <v>412</v>
       </c>
@@ -1800,7 +1883,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="15" customFormat="1">
+    <row r="32" spans="1:52" s="15" customFormat="1">
       <c r="A32" s="10">
         <v>376</v>
       </c>

</xml_diff>